<commit_message>
added updated tables and comparison tables. Updated the methods section and results section to include comparison tables.
</commit_message>
<xml_diff>
--- a/Results/Table_3.xlsx
+++ b/Results/Table_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raed\Documents\R Projects\TTI-AsthmaIR\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5E4BF7-098A-4D8B-9543-42DFB33ADBF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C2606A-9FA3-4718-928D-BCDD380733EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="348" yWindow="3972" windowWidth="10548" windowHeight="11772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>